<commit_message>
remove excess columns and rename
</commit_message>
<xml_diff>
--- a/new_labels.xlsx
+++ b/new_labels.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\个人\smu\Senior\Machine Learning\LABs\lab1\smuml_lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronmatson/smuf17/ml/smuml_lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10068"/>
+    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="15440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -62,46 +68,46 @@
     <t>Do you work remotely?</t>
   </si>
   <si>
-    <t>Number_of_Employees</t>
-  </si>
-  <si>
-    <t>IT Job</t>
-  </si>
-  <si>
-    <t>Past_History</t>
-  </si>
-  <si>
-    <t>Family_History</t>
-  </si>
-  <si>
-    <t>Current_State</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Country_livein</t>
-  </si>
-  <si>
-    <t>Country_work</t>
-  </si>
-  <si>
-    <t>Work_remotely</t>
-  </si>
-  <si>
-    <t>Treatment</t>
-  </si>
-  <si>
-    <t>Employer_Awareness</t>
+    <t>num_employess</t>
+  </si>
+  <si>
+    <t>it_job</t>
+  </si>
+  <si>
+    <t>employer_awareness</t>
+  </si>
+  <si>
+    <t>family_history</t>
+  </si>
+  <si>
+    <t>past_history</t>
+  </si>
+  <si>
+    <t>current_state</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>residence</t>
+  </si>
+  <si>
+    <t>work_location</t>
+  </si>
+  <si>
+    <t>remote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,108 +453,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="102.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="O3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="O6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="O7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="O8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="O9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="O10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="O11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="O12" t="s">
-        <v>21</v>
+      <c r="F12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>